<commit_message>
changes based on consultant feedback
</commit_message>
<xml_diff>
--- a/Risk Chart Updated.xlsx
+++ b/Risk Chart Updated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T4YY4\Documents\GitHub\Individual Project\individualProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D25C902-0E9A-49D0-9679-1264AA586CFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71985F46-E0B1-40E1-8902-7E724D4BE69F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{3DFC32C5-32FC-40DF-8C12-07B23DF2A452}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="47">
   <si>
     <t>Risk Chart</t>
   </si>
@@ -62,30 +62,12 @@
     <t>Consequence Mitigation</t>
   </si>
   <si>
-    <t>Time constraints due to inaccurate time estimations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">To stop myself from running out of time writing the final report, I will complete a rough version of the report alongside building my project. I have also dedicated time at the end of every week to work on the final report and time at the completion of every major objective to complete the report for that section.  </t>
-  </si>
-  <si>
     <t>Revised Assessment after Mitigation</t>
   </si>
   <si>
-    <t xml:space="preserve">If I do run out of time writing my report I could put less emphasis on some of the latter objectives such as Objective 6. Since the most important objectives are completed at the beginning of the project, this should mean that the most important parts of the write-up are also completed at the beginning. Putting less effort inot the latter objectives should not effect the project too badly. </t>
-  </si>
-  <si>
-    <t>To stop myself from running out of time designing, implementing and testing the prototype for the game, I will build the most vital parts of the prototype first. This can be seen in my build plan.</t>
-  </si>
-  <si>
-    <t>Complete Project Report</t>
-  </si>
-  <si>
     <t>Complete Prototype</t>
   </si>
   <si>
-    <t>If I do run out of time building the prototype, I can simply remove some functionality from the latter objectives, such as objective 6. This objective specifically doesn’t offer much in the way of answering my problem to be solved. Removing this will not massively impact my project.</t>
-  </si>
-  <si>
     <t>Main objective of the project, to create a first-person stealth level.</t>
   </si>
   <si>
@@ -110,9 +92,6 @@
     <t>Complete Prototype and Project Report</t>
   </si>
   <si>
-    <t xml:space="preserve">Poor productivity on the project as a whole form me. </t>
-  </si>
-  <si>
     <t xml:space="preserve">To mitigate this risk, I have set aside time every week to allow me to work on my other module IN3005, so that my work on that module does not interfere with this project. Also, within my build plan I have left some leeway at the end of the project to allow me to catch-up with my objectives if i fall behind at any point. </t>
   </si>
   <si>
@@ -138,6 +117,66 @@
   </si>
   <si>
     <t>Since the main parts of the project are completed at the start, I could simply put less emphasis on the latter objectives such as objective 6</t>
+  </si>
+  <si>
+    <t>To stop myself from running out of time writing the final report, I will complete a rough version of the report alongside building my project. I have also dedicated time at the end of every week to work on the final report and time at the completion of every major objective to complete the report for that section. To stop myself from running out of time designing, implementing and testing the prototype for the game, I will build the most vital parts of the prototype first. This can be seen in my build plan.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If I do run out of time on my project I could put less emphasis on some of the latter objectives such as Objective 6. Since the most important objectives are completed at the beginning of the project, this should mean that the most important parts of the write-up and prototype are also conducted at the beginning. Putting less effort into the latter objectives should not affect the project too badly. </t>
+  </si>
+  <si>
+    <t>Complete Project On Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Poor productivity on the project as a whole from me. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Complete Project  </t>
+  </si>
+  <si>
+    <t>Consultant Delays. There may be a risk that my consultant for the project is delayed or unavailable to advise me on my project for any given reason. This could lead to me developing work not in line with their requirements.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To mitigate the risk, I will contact my consultant as regularly as I can so that in the event that they are unavailable I still have some relatively recent feedback. </t>
+  </si>
+  <si>
+    <t>If my consultant is unavailable, I can contact the project team for any short-term guidance or quick queries and I can also consult the project handbook for help. If either of these options has not solved my issues, I can move on to another part of my project and make a note to ask my consultant about the part I was struggling with at the next available opportunity.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Incomprehensive Testing. There is a risk that if the testing of my project is not up to par then bugs or design flaws may be found by my potential beneficiaries after project completion. This could result in my beneficiaries not building upon my prototype due to the potential underlying issues. </t>
+  </si>
+  <si>
+    <t>To mitigate this risk, I will systematically test each implementation during the development phase. This fits in line with my agile methodology approach to the project. What this means is, if there is an issue, I will re-develop this part of the prototype and have it working correctly before moving forward. This should hopefully minimize potential errors in my design/implementation.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In the worst-case scenario, I should let potential beneficiaries know that testing was undertaken by myself during development and due to a lack of time and resources, I was unable to perform thorough quality assurance for my prototype. Going forward, if I want to resolve this, I may have to enlist the help of a QA tester but this is not in the scope of this project. </t>
+  </si>
+  <si>
+    <t>Scope Creep. There is a risk that during development, I may think of new features that may improve my prototype. However, this can lead to time overruns and creates a risk that I may not complete the essential parts of my project before the deadline.</t>
+  </si>
+  <si>
+    <t>To mitigate this risk, I will look over the objectives and requirements for the project regularly and ensure not to add features that are not in my project definition.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To mitigate the consequences of this risk, I could shorten the scope of my total project, especially the last few objectives. In my build plan, the objectives that are most important are completed first, so not including the latter objectives in order to meet time constraints should not affect my prototype too badly. </t>
+  </si>
+  <si>
+    <t>Complete Project</t>
+  </si>
+  <si>
+    <t>Time constraints due to inaccurate time estimations.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generic Objective Specification. There is a risk that my objectives are not well-defined in the project definition. This could lead to some ambiguity in my design and implementation. </t>
+  </si>
+  <si>
+    <t>Mitigating the consequences of this risk is quite difficult within the time frame of this project. However, if I did have more time and by the end of my project I had missed my objectives, then I would have to refactor some parts of my prototype to better fit the requirements.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To mitigate this risk, I will ensure that my objectives are well-defined and unambiguous. It is also important that I regularly check the requirements and objectives so that I am always aware of what the end result should look like. </t>
+  </si>
+  <si>
+    <t>Assessment</t>
   </si>
 </sst>
 </file>
@@ -193,7 +232,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -216,20 +255,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -240,11 +285,20 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="39">
+  <dxfs count="30">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -277,6 +331,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -307,6 +371,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -317,6 +391,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -327,6 +411,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -427,6 +521,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -457,6 +571,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -467,171 +591,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -945,10 +909,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4281B21-9DB5-4D57-9300-08432CBAE3E5}">
-  <dimension ref="A1:K52"/>
+  <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -957,13 +921,14 @@
     <col min="3" max="3" width="10.08984375" customWidth="1"/>
     <col min="4" max="4" width="8.7265625" customWidth="1"/>
     <col min="5" max="5" width="7.08984375" customWidth="1"/>
-    <col min="6" max="7" width="38.1796875" customWidth="1"/>
+    <col min="6" max="6" width="38.1796875" customWidth="1"/>
+    <col min="7" max="7" width="39.08984375" customWidth="1"/>
     <col min="8" max="8" width="10.54296875" customWidth="1"/>
     <col min="9" max="9" width="8.81640625" customWidth="1"/>
-    <col min="10" max="10" width="8" customWidth="1"/>
+    <col min="10" max="10" width="12.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="23.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="23.5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -978,327 +943,390 @@
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
+      <c r="C2" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="1:12" ht="31" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="1:12" ht="188.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="5">
+        <v>2</v>
+      </c>
+      <c r="D4" s="5">
+        <v>5</v>
+      </c>
+      <c r="E4" s="5">
         <v>10</v>
       </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-    </row>
-    <row r="3" spans="1:11" ht="31" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
+      <c r="F4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" s="5">
+        <v>2</v>
+      </c>
+      <c r="I4" s="5">
+        <v>3</v>
+      </c>
+      <c r="J4" s="5">
+        <v>6</v>
+      </c>
+      <c r="K4" s="1"/>
+      <c r="L4" s="6"/>
+    </row>
+    <row r="5" spans="1:12" ht="188.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="5">
+        <v>2</v>
+      </c>
+      <c r="D5" s="5">
+        <v>4</v>
+      </c>
+      <c r="E5" s="5">
+        <v>8</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="5">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="I5" s="5">
+        <v>3</v>
+      </c>
+      <c r="J5" s="5">
+        <v>3</v>
+      </c>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="1:12" ht="145" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="5">
         <v>2</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D6" s="5">
         <v>3</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E6" s="5">
+        <v>6</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="5">
+        <v>2</v>
+      </c>
+      <c r="I6" s="5">
+        <v>2</v>
+      </c>
+      <c r="J6" s="5">
         <v>4</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:12" ht="116" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="5">
+        <v>2</v>
+      </c>
+      <c r="D7" s="5">
         <v>5</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="E7" s="5">
+        <v>10</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="5">
+        <v>1</v>
+      </c>
+      <c r="I7" s="5">
+        <v>3</v>
+      </c>
+      <c r="J7" s="5">
+        <v>3</v>
+      </c>
+      <c r="K7" s="1"/>
+    </row>
+    <row r="8" spans="1:12" ht="58" x14ac:dyDescent="0.35">
+      <c r="A8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="5">
+        <v>2</v>
+      </c>
+      <c r="D8" s="5">
+        <v>3</v>
+      </c>
+      <c r="E8" s="5">
+        <f t="shared" ref="E8:E9" si="0">PRODUCT(C8,D8)</f>
         <v>6</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H3" s="4" t="s">
+      <c r="F8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" s="5">
+        <v>1</v>
+      </c>
+      <c r="I8" s="5">
         <v>3</v>
       </c>
-      <c r="I3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="J3" s="4" t="s">
+      <c r="J8" s="5">
+        <v>3</v>
+      </c>
+      <c r="K8" s="1"/>
+    </row>
+    <row r="9" spans="1:12" ht="58" x14ac:dyDescent="0.35">
+      <c r="A9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="5">
+        <v>2</v>
+      </c>
+      <c r="D9" s="5">
         <v>5</v>
       </c>
-      <c r="K3" s="1"/>
-    </row>
-    <row r="4" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="6">
-        <v>2</v>
-      </c>
-      <c r="D4" s="6">
-        <v>5</v>
-      </c>
-      <c r="E4" s="6">
-        <v>10</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="6">
-        <v>1</v>
-      </c>
-      <c r="I4" s="6">
-        <v>3</v>
-      </c>
-      <c r="J4" s="6">
-        <v>3</v>
-      </c>
-      <c r="K4" s="1"/>
-    </row>
-    <row r="5" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="6">
-        <v>2</v>
-      </c>
-      <c r="D5" s="6">
-        <v>5</v>
-      </c>
-      <c r="E5" s="6">
-        <v>10</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5" s="6">
-        <v>2</v>
-      </c>
-      <c r="I5" s="6">
-        <v>3</v>
-      </c>
-      <c r="J5" s="6">
-        <v>6</v>
-      </c>
-      <c r="K5" s="1"/>
-    </row>
-    <row r="6" spans="1:11" ht="188.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="6">
-        <v>2</v>
-      </c>
-      <c r="D6" s="6">
-        <v>4</v>
-      </c>
-      <c r="E6" s="6">
-        <v>8</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H6" s="6">
-        <v>1</v>
-      </c>
-      <c r="I6" s="6">
-        <v>3</v>
-      </c>
-      <c r="J6" s="6">
-        <v>3</v>
-      </c>
-      <c r="K6" s="1"/>
-    </row>
-    <row r="7" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="6">
-        <v>2</v>
-      </c>
-      <c r="D7" s="6">
-        <v>3</v>
-      </c>
-      <c r="E7" s="6">
-        <v>6</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H7" s="6">
-        <v>2</v>
-      </c>
-      <c r="I7" s="6">
-        <v>2</v>
-      </c>
-      <c r="J7" s="6">
-        <v>4</v>
-      </c>
-      <c r="K7" s="1"/>
-    </row>
-    <row r="8" spans="1:11" ht="116" x14ac:dyDescent="0.35">
-      <c r="A8" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="6">
-        <v>2</v>
-      </c>
-      <c r="D8" s="6">
-        <v>5</v>
-      </c>
-      <c r="E8" s="6">
-        <v>10</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="H8" s="6">
-        <v>1</v>
-      </c>
-      <c r="I8" s="6">
-        <v>3</v>
-      </c>
-      <c r="J8" s="6">
-        <v>3</v>
-      </c>
-      <c r="K8" s="1"/>
-    </row>
-    <row r="9" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A9" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="6">
-        <v>2</v>
-      </c>
-      <c r="D9" s="6">
-        <v>3</v>
-      </c>
-      <c r="E9" s="6">
-        <f t="shared" ref="E9:E10" si="0">PRODUCT(C9,D9)</f>
-        <v>6</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H9" s="6">
-        <v>1</v>
-      </c>
-      <c r="I9" s="6">
-        <v>3</v>
-      </c>
-      <c r="J9" s="6">
-        <v>3</v>
-      </c>
-      <c r="K9" s="1"/>
-    </row>
-    <row r="10" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A10" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="6">
-        <v>2</v>
-      </c>
-      <c r="D10" s="6">
-        <v>5</v>
-      </c>
-      <c r="E10" s="6">
+      <c r="E9" s="5">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" s="5">
+        <v>1</v>
+      </c>
+      <c r="I9" s="5">
+        <v>4</v>
+      </c>
+      <c r="J9" s="5">
+        <v>4</v>
+      </c>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="10" spans="1:12" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="C10" s="5">
+        <v>2</v>
+      </c>
+      <c r="D10" s="5">
+        <v>2</v>
+      </c>
+      <c r="E10" s="5">
+        <v>4</v>
+      </c>
+      <c r="F10" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="H10" s="6">
+      <c r="G10" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H10" s="5">
         <v>1</v>
       </c>
-      <c r="I10" s="6">
-        <v>4</v>
-      </c>
-      <c r="J10" s="6">
-        <v>4</v>
+      <c r="I10" s="5">
+        <v>1</v>
+      </c>
+      <c r="J10" s="5">
+        <v>1</v>
       </c>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
+    <row r="11" spans="1:12" ht="145" x14ac:dyDescent="0.35">
+      <c r="A11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="5">
+        <v>3</v>
+      </c>
+      <c r="D11" s="5">
+        <v>3</v>
+      </c>
+      <c r="E11" s="5">
+        <v>9</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H11" s="5">
+        <v>2</v>
+      </c>
+      <c r="I11" s="5">
+        <v>3</v>
+      </c>
+      <c r="J11" s="5">
+        <v>6</v>
+      </c>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
+    <row r="12" spans="1:12" ht="116" x14ac:dyDescent="0.35">
+      <c r="A12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="5">
+        <v>2</v>
+      </c>
+      <c r="D12" s="5">
+        <v>3</v>
+      </c>
+      <c r="E12" s="5">
+        <v>6</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H12" s="5">
+        <v>1</v>
+      </c>
+      <c r="I12" s="5">
+        <v>2</v>
+      </c>
+      <c r="J12" s="5">
+        <v>2</v>
+      </c>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
+    <row r="13" spans="1:12" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="5">
+        <v>2</v>
+      </c>
+      <c r="D13" s="5">
+        <v>3</v>
+      </c>
+      <c r="E13" s="5">
+        <v>6</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H13" s="5">
+        <v>1</v>
+      </c>
+      <c r="I13" s="5">
+        <v>3</v>
+      </c>
+      <c r="J13" s="5">
+        <v>3</v>
+      </c>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1311,7 +1339,7 @@
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1324,7 +1352,7 @@
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1792,125 +1820,145 @@
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A52" s="1"/>
-      <c r="B52" s="1"/>
-      <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
-      <c r="E52" s="1"/>
-      <c r="F52" s="1"/>
-      <c r="G52" s="1"/>
-      <c r="H52" s="1"/>
-      <c r="I52" s="1"/>
-      <c r="J52" s="1"/>
-      <c r="K52" s="1"/>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="C4:D8 H4:I8">
-    <cfRule type="cellIs" dxfId="28" priority="24" operator="between">
+  <mergeCells count="2">
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="H2:J2"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C4:D7 H4:I7">
+    <cfRule type="cellIs" dxfId="29" priority="30" operator="between">
+      <formula>4</formula>
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="31" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="27" priority="32" operator="between">
       <formula>1</formula>
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="23" operator="equal">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4:E7 J4:J9">
+    <cfRule type="cellIs" dxfId="26" priority="27" operator="between">
+      <formula>18</formula>
+      <formula>25</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="28" operator="between">
+      <formula>8</formula>
+      <formula>17</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="29" operator="between">
+      <formula>0</formula>
+      <formula>7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8:D8">
+    <cfRule type="cellIs" dxfId="23" priority="24" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="22" operator="between">
+    <cfRule type="cellIs" dxfId="22" priority="25" operator="between">
       <formula>4</formula>
       <formula>5</formula>
     </cfRule>
+    <cfRule type="cellIs" dxfId="21" priority="26" operator="between">
+      <formula>1</formula>
+      <formula>2</formula>
+    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E4:E8 J4:J10">
-    <cfRule type="cellIs" dxfId="18" priority="21" operator="between">
+  <conditionalFormatting sqref="E8">
+    <cfRule type="cellIs" dxfId="20" priority="21" operator="between">
+      <formula>18</formula>
+      <formula>25</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="22" operator="between">
+      <formula>8</formula>
+      <formula>17</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="23" operator="between">
+      <formula>1</formula>
+      <formula>7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C9:D9">
+    <cfRule type="cellIs" dxfId="17" priority="18" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="19" operator="between">
+      <formula>4</formula>
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="20" operator="between">
+      <formula>1</formula>
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E9">
+    <cfRule type="cellIs" dxfId="14" priority="15" operator="between">
+      <formula>18</formula>
+      <formula>25</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="16" operator="between">
+      <formula>8</formula>
+      <formula>17</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="17" operator="between">
+      <formula>1</formula>
+      <formula>7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H8:I8">
+    <cfRule type="cellIs" dxfId="11" priority="12" operator="between">
+      <formula>4</formula>
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="13" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="14" operator="between">
+      <formula>1</formula>
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H9:I9">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="between">
+      <formula>4</formula>
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="10" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="11" operator="between">
+      <formula>1</formula>
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C10:D13 H10:I13">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="7" operator="between">
+      <formula>4</formula>
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="8" operator="between">
+      <formula>0</formula>
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E10:E13 J10:J13">
+    <cfRule type="cellIs" dxfId="2" priority="5" operator="between">
       <formula>0</formula>
       <formula>7</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="20" operator="between">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J10:J13 E10:E13">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
       <formula>8</formula>
       <formula>17</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="19" operator="between">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="between">
       <formula>18</formula>
       <formula>25</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C9:D9">
-    <cfRule type="cellIs" dxfId="15" priority="16" operator="equal">
-      <formula>3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="17" operator="between">
-      <formula>4</formula>
-      <formula>5</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="18" operator="between">
-      <formula>1</formula>
-      <formula>2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E9">
-    <cfRule type="cellIs" dxfId="12" priority="13" operator="between">
-      <formula>18</formula>
-      <formula>25</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="14" operator="between">
-      <formula>8</formula>
-      <formula>17</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="15" operator="between">
-      <formula>1</formula>
-      <formula>7</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C10:D10">
-    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
-      <formula>3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="between">
-      <formula>4</formula>
-      <formula>5</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="12" operator="between">
-      <formula>1</formula>
-      <formula>2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E10">
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="between">
-      <formula>18</formula>
-      <formula>25</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="between">
-      <formula>8</formula>
-      <formula>17</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="between">
-      <formula>1</formula>
-      <formula>7</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H9:I9">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="between">
-      <formula>4</formula>
-      <formula>5</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
-      <formula>3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="between">
-      <formula>1</formula>
-      <formula>2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H10:I10">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="between">
-      <formula>4</formula>
-      <formula>5</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
-      <formula>3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="between">
-      <formula>1</formula>
-      <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>